<commit_message>
chore: update xlsx format
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\excel_to_ipxact\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanjt01\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBA8DBC-0533-4F34-A5D9-467AB976F31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9B5CA1-E1A2-4984-88CC-D80EC9D4441A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{CE17D36E-8982-7C47-A020-5E6655990FA9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{CE17D36E-8982-7C47-A020-5E6655990FA9}"/>
   </bookViews>
   <sheets>
     <sheet name="version" sheetId="4" r:id="rId1"/>
@@ -23,21 +23,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="55">
   <si>
     <t>BLOCK</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -87,163 +81,175 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>ATTRIBUTE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEFAULT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>example</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DESCIPTION</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>block0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>block1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>field0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[31:0]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[7:0]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x1234</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[15:8]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[23:16]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[31:24]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>field1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W1C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[31:16]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[15:0]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>example.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reserved1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reserved0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg0.field0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>WIDTH</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ATTRIBUTE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DEFAULT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>example</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DESCIPTION</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>block0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>block1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x1000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0xc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>field0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[31:0]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[7:0]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RW</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x1234</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[15:8]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[23:16]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[31:24]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>field1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>W1C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[31:16]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[15:0]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TAG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VALUE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>example.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rega{n}, n=0~3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>regb{n}, n=0~3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reserved</t>
+    <t>rega{n}, n=range(3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>regb{n}, n=range(0, 2, 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rega{n}, n=range(1, 3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>regc{n}, n=range(3)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -290,7 +296,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -298,9 +304,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -640,62 +643,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725A8A21-6CE1-5947-A0CB-208E9DE2092A}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3"/>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -712,7 +703,7 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.453125" style="1" bestFit="1" customWidth="1"/>
@@ -731,29 +722,29 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -764,22 +755,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08ACDB31-7888-5646-9BBF-168BB80551E6}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.36328125" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -796,13 +786,13 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
@@ -810,217 +800,235 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="1">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="1">
-        <v>32</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" s="1">
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
       </c>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="1">
         <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
       </c>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1">
         <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
       </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1">
         <v>8</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
       </c>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E7" s="1">
         <v>32</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
       </c>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E8" s="1">
         <v>32</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
       </c>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1">
+        <v>32</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="1">
-        <v>32</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="B10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="E10" s="1">
         <v>16</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G10" s="1">
         <v>0</v>
       </c>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" s="1">
         <v>16</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
       </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H13" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1037,19 +1045,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FF57BE-6DA6-9A46-A269-C97099FCCA20}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7265625" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.81640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="1" bestFit="1" customWidth="1"/>
@@ -1069,13 +1077,13 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
@@ -1083,102 +1091,102 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="1">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="1">
-        <v>32</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" s="1">
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="1">
         <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1">
         <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1">
         <v>8</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -1186,22 +1194,22 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E7" s="1">
         <v>32</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
@@ -1209,22 +1217,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E8" s="1">
         <v>32</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
@@ -1232,77 +1240,122 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1">
+        <v>32</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="1">
-        <v>32</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="B10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="E10" s="1">
         <v>16</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G10" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" s="1">
         <v>16</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
       </c>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="1">
+        <v>16</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="1">
+        <v>16</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>